<commit_message>
Merge #225 - #241
</commit_message>
<xml_diff>
--- a/WEBAPP/Uploads/Template/MIS/MISS01TP001.xlsx
+++ b/WEBAPP/Uploads/Template/MIS/MISS01TP001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\po.klinmala\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Senior\SDLC\sdmsbitbucket\WEBAPP\Uploads\Template\MIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06549F07-5D93-4C44-90FC-9784CF7E98F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D9CC88-EF3C-4EB9-BE4A-9509AFE1F527}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="216" yWindow="1896" windowWidth="17292" windowHeight="8964" activeTab="1" xr2:uid="{BA1FD271-BACF-498B-9238-A4F6283D44C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BA1FD271-BACF-498B-9238-A4F6283D44C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>No</t>
   </si>
@@ -131,12 +131,6 @@
   </si>
   <si>
     <t>T001OOI</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>swqd</t>
   </si>
   <si>
     <t>dqwdqw</t>
@@ -615,15 +609,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BABC95-B0F8-4889-839D-CA92BB42C69C}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -640,82 +634,76 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="U1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="V1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="W1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="X1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Z1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AA1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -741,19 +729,19 @@
         <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>32</v>
@@ -762,19 +750,19 @@
         <v>32</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>44</v>
@@ -782,18 +770,12 @@
       <c r="V2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -805,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E8CF74-46FC-4FBF-989D-DC0B8FA828F1}">
   <dimension ref="D5:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -820,10 +802,10 @@
         <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>0</v>
@@ -835,10 +817,10 @@
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="3">
         <v>2019</v>
@@ -853,10 +835,10 @@
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D7" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7" s="3">
         <v>2019</v>
@@ -865,19 +847,19 @@
         <v>2</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>3</v>
@@ -898,7 +880,7 @@
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2"/>
       <c r="H10" s="7" t="s">
@@ -977,7 +959,7 @@
         <v>13</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J18" s="6"/>
     </row>
@@ -986,7 +968,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J19" s="6"/>
     </row>
@@ -995,7 +977,7 @@
         <v>15</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J20" s="6"/>
     </row>
@@ -1004,7 +986,7 @@
         <v>16</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J21" s="6"/>
     </row>
@@ -1031,7 +1013,7 @@
         <v>19</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J24" s="6"/>
     </row>

</xml_diff>